<commit_message>
Added screenshots for Question 3
</commit_message>
<xml_diff>
--- a/Results Table - Heuristic.xlsx
+++ b/Results Table - Heuristic.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnn\Desktop\Final Year\AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC127F90-9255-437B-BB96-3AECEF41ABC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5452FC9F-747B-4E79-8F56-CD68190DCFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{45322249-8D49-473F-980B-78B6BDAAE694}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{45322249-8D49-473F-980B-78B6BDAAE694}"/>
   </bookViews>
   <sheets>
     <sheet name="Path Plan Tests" sheetId="2" r:id="rId1"/>
     <sheet name="Dispatch Tests" sheetId="1" r:id="rId2"/>
+    <sheet name="Question 3 Tests" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -178,10 +179,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -198,6 +199,187 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>591228</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38322</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A071CA06-ADC3-4AE2-9DA8-F6F67D1AADB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="161925"/>
+          <a:ext cx="4858428" cy="1590897"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>124608</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>171737</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E71F6019-6C4D-480A-AEC3-FF438D2BA388}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1924050"/>
+          <a:ext cx="5611008" cy="2057687"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>86333</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19265</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CD8B81C-B7B4-401D-A70C-CD21945642FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="0"/>
+          <a:ext cx="4353533" cy="1543265"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>181682</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114692</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07D03B1A-3C83-400B-963D-27069AF5281A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6086475" y="1876425"/>
+          <a:ext cx="5068007" cy="2810267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -511,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5768E6-7FD8-474C-9BAC-BC6300944EF4}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J62" sqref="J62"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +796,7 @@
       <c r="L2" s="1">
         <v>1</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="8">
         <v>52.22</v>
       </c>
       <c r="N2" s="1"/>
@@ -2205,7 +2387,7 @@
       </c>
     </row>
     <row r="67" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="K67" s="8" t="s">
+      <c r="K67" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2213,4 +2395,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B592C005-65B5-45AD-8A57-AD2A7E099D28}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final Version for all Test Data
</commit_message>
<xml_diff>
--- a/Results Table - Heuristic.xlsx
+++ b/Results Table - Heuristic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnn\Desktop\Final Year\AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF915F2D-8E0E-4671-83D4-9E2E8F9B3CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D52FA2F-29C8-49D9-A32A-41B9E6B8AE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{45322249-8D49-473F-980B-78B6BDAAE694}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{45322249-8D49-473F-980B-78B6BDAAE694}"/>
   </bookViews>
   <sheets>
     <sheet name="Path Plan Tests" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="34">
   <si>
     <t>AccountWeight</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Average Return for Taxi</t>
   </si>
   <si>
-    <t>* With traffic on</t>
-  </si>
-  <si>
     <t>* Run on the right is origin with A* search</t>
   </si>
   <si>
@@ -137,12 +134,18 @@
   <si>
     <t>2)</t>
   </si>
+  <si>
+    <t>* With traffic on and traffic probability</t>
+  </si>
+  <si>
+    <t>* With traffic on and no probability</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,13 +157,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -312,24 +308,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -828,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEBE87FE-52A8-4C28-8B86-A46768933928}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,6 +1189,9 @@
       <c r="G17" s="9" t="s">
         <v>17</v>
       </c>
+      <c r="H17" s="18" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -1201,17 +1200,17 @@
       </c>
       <c r="C18" s="5">
         <f>(D18*10)/4</f>
-        <v>111.1</v>
+        <v>103.05</v>
       </c>
       <c r="D18" s="5">
-        <v>44.44</v>
+        <v>41.22</v>
       </c>
       <c r="E18" s="5">
         <f>SUM(C18, D18)</f>
-        <v>155.54</v>
+        <v>144.26999999999998</v>
       </c>
       <c r="F18" s="5">
-        <v>424</v>
+        <v>446</v>
       </c>
       <c r="G18" s="5">
         <v>0</v>
@@ -1224,17 +1223,17 @@
       </c>
       <c r="C19" s="5">
         <f t="shared" ref="C19:C22" si="4">(D19*10)/4</f>
-        <v>210.55</v>
+        <v>92.775000000000006</v>
       </c>
       <c r="D19" s="5">
-        <v>84.22</v>
+        <v>37.11</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" ref="E19:E22" si="5">SUM(C19, D19)</f>
-        <v>294.77</v>
+        <v>129.88499999999999</v>
       </c>
       <c r="F19" s="5">
-        <v>425</v>
+        <v>435</v>
       </c>
       <c r="G19" s="5">
         <v>0</v>
@@ -1247,17 +1246,17 @@
       </c>
       <c r="C20" s="5">
         <f t="shared" si="4"/>
-        <v>156.67500000000001</v>
+        <v>80.824999999999989</v>
       </c>
       <c r="D20" s="5">
-        <v>62.67</v>
+        <v>32.33</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="5"/>
-        <v>219.34500000000003</v>
+        <v>113.15499999999999</v>
       </c>
       <c r="F20" s="5">
-        <v>422</v>
+        <v>435</v>
       </c>
       <c r="G20" s="5">
         <v>0</v>
@@ -1270,17 +1269,17 @@
       </c>
       <c r="C21" s="5">
         <f t="shared" si="4"/>
-        <v>115</v>
+        <v>97.775000000000006</v>
       </c>
       <c r="D21" s="5">
-        <v>46</v>
+        <v>39.11</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="5"/>
-        <v>161</v>
+        <v>136.88499999999999</v>
       </c>
       <c r="F21" s="5">
-        <v>445</v>
+        <v>420</v>
       </c>
       <c r="G21" s="5">
         <v>0</v>
@@ -1293,17 +1292,17 @@
       </c>
       <c r="C22" s="11">
         <f t="shared" si="4"/>
-        <v>175</v>
+        <v>45.55</v>
       </c>
       <c r="D22" s="11">
-        <v>70</v>
+        <v>18.22</v>
       </c>
       <c r="E22" s="11">
         <f t="shared" si="5"/>
-        <v>245</v>
+        <v>63.769999999999996</v>
       </c>
       <c r="F22" s="11">
-        <v>406</v>
+        <v>449</v>
       </c>
       <c r="G22" s="11">
         <v>0</v>
@@ -1316,19 +1315,19 @@
       </c>
       <c r="C23" s="6">
         <f>SUM(C18:C22)/5</f>
-        <v>153.66500000000002</v>
+        <v>83.99499999999999</v>
       </c>
       <c r="D23" s="6">
         <f>SUM(D18:D22)/5</f>
-        <v>61.465999999999994</v>
+        <v>33.597999999999999</v>
       </c>
       <c r="E23" s="6">
         <f>SUM(E18:E22)/5</f>
-        <v>215.131</v>
+        <v>117.59299999999999</v>
       </c>
       <c r="F23" s="6">
         <f>SUM(F18:F22)/5</f>
-        <v>424.4</v>
+        <v>437</v>
       </c>
       <c r="G23" s="7">
         <f>SUM(G18:G22)/5</f>
@@ -1357,8 +1356,8 @@
       <c r="G25" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="12" t="s">
-        <v>26</v>
+      <c r="H25" s="18" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1391,17 +1390,17 @@
       </c>
       <c r="C27" s="5">
         <f t="shared" ref="C27:C30" si="6">(D27*10)/4</f>
-        <v>129.72499999999999</v>
+        <v>107.22499999999999</v>
       </c>
       <c r="D27" s="5">
-        <v>51.89</v>
+        <v>42.89</v>
       </c>
       <c r="E27" s="5">
         <f t="shared" ref="E27:E30" si="7">SUM(C27, D27)</f>
-        <v>181.61500000000001</v>
+        <v>150.11500000000001</v>
       </c>
       <c r="F27" s="5">
-        <v>448</v>
+        <v>431</v>
       </c>
       <c r="G27" s="5">
         <v>0</v>
@@ -1420,7 +1419,7 @@
         <v>49.56</v>
       </c>
       <c r="E28" s="5">
-        <f t="shared" si="7"/>
+        <f>SUM(C28, D28)</f>
         <v>173.46</v>
       </c>
       <c r="F28" s="5">
@@ -1437,14 +1436,14 @@
       </c>
       <c r="C29" s="5">
         <f t="shared" si="6"/>
-        <v>106.67500000000001</v>
+        <v>121.67500000000001</v>
       </c>
       <c r="D29" s="5">
-        <v>42.67</v>
+        <v>48.67</v>
       </c>
       <c r="E29" s="5">
         <f t="shared" si="7"/>
-        <v>149.34500000000003</v>
+        <v>170.34500000000003</v>
       </c>
       <c r="F29" s="5">
         <v>430</v>
@@ -1483,19 +1482,19 @@
       </c>
       <c r="C31" s="6">
         <f>SUM(C26:C30)/5</f>
-        <v>114.89500000000001</v>
+        <v>113.39500000000001</v>
       </c>
       <c r="D31" s="6">
         <f>SUM(D26:D30)/5</f>
-        <v>45.958000000000006</v>
+        <v>45.358000000000004</v>
       </c>
       <c r="E31" s="6">
         <f>SUM(E26:E30)/5</f>
-        <v>160.85300000000001</v>
+        <v>158.75300000000001</v>
       </c>
       <c r="F31" s="6">
         <f>SUM(F26:F30)/5</f>
-        <v>427</v>
+        <v>423.6</v>
       </c>
       <c r="G31" s="7">
         <f>SUM(G26:G30)/5</f>
@@ -1504,6 +1503,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1511,7 +1511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5768E6-7FD8-474C-9BAC-BC6300944EF4}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -1536,7 +1536,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>5</v>
@@ -1610,8 +1610,8 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
-      <c r="K2" s="17" t="s">
-        <v>27</v>
+      <c r="K2" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="L2" s="5">
         <v>1</v>
@@ -1749,15 +1749,15 @@
       <c r="G6" s="5">
         <v>128.22</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="13">
         <f>SUM(G2:G6)/5</f>
         <v>111.52799999999999</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="13">
         <f>MAX(G2:G6)</f>
         <v>128.22</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="13">
         <f>MIN(G2:G6)</f>
         <v>100.55</v>
       </c>
@@ -1768,151 +1768,151 @@
       <c r="M6" s="5">
         <v>62.66</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="13">
         <f>SUM(M2:M6)/5</f>
         <v>67.33</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="13">
         <f>MAX(M2:M6)</f>
         <v>85.22</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="13">
         <f>MIN(M2:M6)</f>
         <v>52.22</v>
       </c>
-      <c r="Q6" s="14">
+      <c r="Q6" s="13">
         <v>413</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="13">
-        <v>1</v>
-      </c>
-      <c r="C7" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="D7" s="13">
-        <v>1</v>
-      </c>
-      <c r="E7" s="13">
-        <v>1</v>
-      </c>
-      <c r="F7" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G7" s="15">
+      <c r="B7" s="12">
+        <v>1</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="12">
+        <v>1</v>
+      </c>
+      <c r="E7" s="12">
+        <v>1</v>
+      </c>
+      <c r="F7" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="14">
         <v>112.77</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <v>2</v>
       </c>
-      <c r="C8" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="D8" s="13">
-        <v>1</v>
-      </c>
-      <c r="E8" s="13">
-        <v>1</v>
-      </c>
-      <c r="F8" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="15">
+      <c r="C8" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="12">
+        <v>1</v>
+      </c>
+      <c r="E8" s="12">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="14">
         <v>108.66</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <v>3</v>
       </c>
-      <c r="C9" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="D9" s="13">
-        <v>1</v>
-      </c>
-      <c r="E9" s="13">
-        <v>1</v>
-      </c>
-      <c r="F9" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G9" s="15">
+      <c r="C9" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="12">
+        <v>1</v>
+      </c>
+      <c r="E9" s="12">
+        <v>1</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="14">
         <v>95.33</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <v>4</v>
       </c>
-      <c r="C10" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="13">
-        <v>1</v>
-      </c>
-      <c r="E10" s="13">
-        <v>1</v>
-      </c>
-      <c r="F10" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G10" s="15">
+      <c r="C10" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1</v>
+      </c>
+      <c r="E10" s="12">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="14">
         <v>96.44</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <v>5</v>
       </c>
-      <c r="C11" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="D11" s="13">
-        <v>1</v>
-      </c>
-      <c r="E11" s="13">
-        <v>1</v>
-      </c>
-      <c r="F11" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G11" s="15">
+      <c r="C11" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1</v>
+      </c>
+      <c r="E11" s="12">
+        <v>1</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="14">
         <v>103.44</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="13">
         <f>SUM(G7:G11)/5</f>
         <v>103.328</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="13">
         <f>MAX(G7:G11)</f>
         <v>112.77</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="13">
         <f>MIN(G7:G11)</f>
         <v>95.33</v>
       </c>
@@ -2054,133 +2054,133 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="15">
-        <v>1</v>
-      </c>
-      <c r="C17" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D17" s="15">
-        <v>1</v>
-      </c>
-      <c r="E17" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F17" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="G17" s="15">
+      <c r="B17" s="14">
+        <v>1</v>
+      </c>
+      <c r="C17" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="14">
+        <v>1</v>
+      </c>
+      <c r="E17" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="14">
         <v>109.11</v>
       </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <v>2</v>
       </c>
-      <c r="C18" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D18" s="15">
-        <v>1</v>
-      </c>
-      <c r="E18" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F18" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="G18" s="15">
+      <c r="C18" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="14">
+        <v>1</v>
+      </c>
+      <c r="E18" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="14">
         <v>118.88</v>
       </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="15">
+      <c r="B19" s="14">
         <v>3</v>
       </c>
-      <c r="C19" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D19" s="15">
-        <v>1</v>
-      </c>
-      <c r="E19" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F19" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="G19" s="15">
+      <c r="C19" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="14">
+        <v>1</v>
+      </c>
+      <c r="E19" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F19" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="G19" s="14">
         <v>101.55</v>
       </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="15">
+      <c r="B20" s="14">
         <v>4</v>
       </c>
-      <c r="C20" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D20" s="15">
-        <v>1</v>
-      </c>
-      <c r="E20" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F20" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="G20" s="15">
+      <c r="C20" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="14">
+        <v>1</v>
+      </c>
+      <c r="E20" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="14">
         <v>99.11</v>
       </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="15">
+      <c r="B21" s="14">
         <v>5</v>
       </c>
-      <c r="C21" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D21" s="15">
-        <v>1</v>
-      </c>
-      <c r="E21" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F21" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="G21" s="15">
+      <c r="C21" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="14">
+        <v>1</v>
+      </c>
+      <c r="E21" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="14">
         <v>113.77</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="13">
         <f>SUM(G17:G21)/5</f>
         <v>108.48400000000001</v>
       </c>
-      <c r="I21" s="14">
+      <c r="I21" s="13">
         <f>MAX(G17:G21)</f>
         <v>118.88</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="13">
         <f>MIN(G17:G21)</f>
         <v>99.11</v>
       </c>
@@ -2306,15 +2306,15 @@
       <c r="G26" s="5">
         <v>114.11</v>
       </c>
-      <c r="H26" s="14">
+      <c r="H26" s="13">
         <f>SUM(G22:G26)/5</f>
         <v>114.532</v>
       </c>
-      <c r="I26" s="14">
+      <c r="I26" s="13">
         <f>MAX(G22:G26)</f>
         <v>117</v>
       </c>
-      <c r="J26" s="14">
+      <c r="J26" s="13">
         <f>MIN(G22:G26)</f>
         <v>111.44</v>
       </c>
@@ -2322,133 +2322,133 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="15">
-        <v>1</v>
-      </c>
-      <c r="C27" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D27" s="15">
-        <v>1</v>
-      </c>
-      <c r="E27" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F27" s="15">
+      <c r="B27" s="14">
+        <v>1</v>
+      </c>
+      <c r="C27" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="14">
+        <v>1</v>
+      </c>
+      <c r="E27" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F27" s="14">
         <v>0.1</v>
       </c>
-      <c r="G27" s="13">
+      <c r="G27" s="12">
         <v>108.88</v>
       </c>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
       <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="15">
+      <c r="B28" s="14">
         <v>2</v>
       </c>
-      <c r="C28" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D28" s="15">
-        <v>1</v>
-      </c>
-      <c r="E28" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F28" s="15">
+      <c r="C28" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="14">
+        <v>1</v>
+      </c>
+      <c r="E28" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F28" s="14">
         <v>0.1</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G28" s="12">
         <v>109.22</v>
       </c>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="15">
+      <c r="B29" s="14">
         <v>3</v>
       </c>
-      <c r="C29" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D29" s="15">
-        <v>1</v>
-      </c>
-      <c r="E29" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F29" s="15">
+      <c r="C29" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="14">
+        <v>1</v>
+      </c>
+      <c r="E29" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F29" s="14">
         <v>0.1</v>
       </c>
-      <c r="G29" s="13">
+      <c r="G29" s="12">
         <v>110.88</v>
       </c>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
       <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="15">
+      <c r="B30" s="14">
         <v>4</v>
       </c>
-      <c r="C30" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D30" s="15">
-        <v>1</v>
-      </c>
-      <c r="E30" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F30" s="15">
+      <c r="C30" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="14">
+        <v>1</v>
+      </c>
+      <c r="E30" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F30" s="14">
         <v>0.1</v>
       </c>
-      <c r="G30" s="15">
+      <c r="G30" s="14">
         <v>103.33</v>
       </c>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
       <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="15">
+      <c r="B31" s="14">
         <v>5</v>
       </c>
-      <c r="C31" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D31" s="15">
-        <v>1</v>
-      </c>
-      <c r="E31" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F31" s="15">
+      <c r="C31" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="14">
+        <v>1</v>
+      </c>
+      <c r="E31" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F31" s="14">
         <v>0.1</v>
       </c>
-      <c r="G31" s="13">
+      <c r="G31" s="12">
         <v>102.22</v>
       </c>
-      <c r="H31" s="14">
+      <c r="H31" s="13">
         <f>SUM(G27:G31)/5</f>
         <v>106.90599999999999</v>
       </c>
-      <c r="I31" s="14">
+      <c r="I31" s="13">
         <f>MAX(G27:G31)</f>
         <v>110.88</v>
       </c>
-      <c r="J31" s="14">
+      <c r="J31" s="13">
         <f>MIN(G27:G31)</f>
         <v>102.22</v>
       </c>
@@ -2576,15 +2576,15 @@
       <c r="G36" s="5">
         <v>107.66</v>
       </c>
-      <c r="H36" s="14">
+      <c r="H36" s="13">
         <f>SUM(G32:G36)/5</f>
         <v>102.92999999999999</v>
       </c>
-      <c r="I36" s="14">
+      <c r="I36" s="13">
         <f>MAX(G32:G36)</f>
         <v>109.55</v>
       </c>
-      <c r="J36" s="14">
+      <c r="J36" s="13">
         <f>MIN(G32:G36)</f>
         <v>95.22</v>
       </c>
@@ -2592,133 +2592,133 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="15">
-        <v>1</v>
-      </c>
-      <c r="C37" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D37" s="15">
+      <c r="B37" s="14">
+        <v>1</v>
+      </c>
+      <c r="C37" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D37" s="14">
         <v>0.75</v>
       </c>
-      <c r="E37" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F37" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="G37" s="13">
+      <c r="E37" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F37" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G37" s="12">
         <v>98.11</v>
       </c>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
       <c r="K37" s="1"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="15">
+      <c r="B38" s="14">
         <v>2</v>
       </c>
-      <c r="C38" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D38" s="15">
+      <c r="C38" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D38" s="14">
         <v>0.75</v>
       </c>
-      <c r="E38" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F38" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="G38" s="13">
+      <c r="E38" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F38" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G38" s="12">
         <v>126</v>
       </c>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="15">
+      <c r="B39" s="14">
         <v>3</v>
       </c>
-      <c r="C39" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D39" s="15">
+      <c r="C39" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D39" s="14">
         <v>0.75</v>
       </c>
-      <c r="E39" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F39" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="G39" s="13">
+      <c r="E39" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F39" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G39" s="12">
         <v>102.55</v>
       </c>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="13"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
       <c r="K39" s="1"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="15">
+      <c r="B40" s="14">
         <v>4</v>
       </c>
-      <c r="C40" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D40" s="15">
+      <c r="C40" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D40" s="14">
         <v>0.75</v>
       </c>
-      <c r="E40" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F40" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="G40" s="13">
+      <c r="E40" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F40" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G40" s="12">
         <v>110.77</v>
       </c>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
       <c r="K40" s="1"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="15">
+      <c r="B41" s="14">
         <v>5</v>
       </c>
-      <c r="C41" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D41" s="15">
+      <c r="C41" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D41" s="14">
         <v>0.75</v>
       </c>
-      <c r="E41" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F41" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="G41" s="13">
+      <c r="E41" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F41" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G41" s="12">
         <v>109.33</v>
       </c>
-      <c r="H41" s="14">
+      <c r="H41" s="13">
         <f>SUM(G37:G41)/5</f>
         <v>109.352</v>
       </c>
-      <c r="I41" s="14">
+      <c r="I41" s="13">
         <f>MAX(G37:G41)</f>
         <v>126</v>
       </c>
-      <c r="J41" s="14">
+      <c r="J41" s="13">
         <f>MIN(G37:G41)</f>
         <v>98.11</v>
       </c>
@@ -2846,15 +2846,15 @@
       <c r="G46" s="5">
         <v>102.11</v>
       </c>
-      <c r="H46" s="14">
+      <c r="H46" s="13">
         <f>SUM(G42:G46)/5</f>
         <v>91.26</v>
       </c>
-      <c r="I46" s="14">
+      <c r="I46" s="13">
         <f>MAX(G42:G46)</f>
         <v>102.11</v>
       </c>
-      <c r="J46" s="14">
+      <c r="J46" s="13">
         <f>MIN(G42:G46)</f>
         <v>78.88</v>
       </c>
@@ -2862,133 +2862,133 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="B47" s="15">
-        <v>1</v>
-      </c>
-      <c r="C47" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="D47" s="15">
+      <c r="B47" s="14">
+        <v>1</v>
+      </c>
+      <c r="C47" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D47" s="14">
         <v>0.75</v>
       </c>
-      <c r="E47" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F47" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="G47" s="13">
+      <c r="E47" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F47" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G47" s="12">
         <v>107.77</v>
       </c>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="13"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
       <c r="K47" s="1"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-      <c r="B48" s="15">
+      <c r="B48" s="14">
         <v>2</v>
       </c>
-      <c r="C48" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="D48" s="15">
+      <c r="C48" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D48" s="14">
         <v>0.75</v>
       </c>
-      <c r="E48" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F48" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="G48" s="13">
+      <c r="E48" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F48" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G48" s="12">
         <v>103.11</v>
       </c>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
-      <c r="J48" s="13"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
       <c r="K48" s="1"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="B49" s="15">
+      <c r="B49" s="14">
         <v>3</v>
       </c>
-      <c r="C49" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="D49" s="15">
+      <c r="C49" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D49" s="14">
         <v>0.75</v>
       </c>
-      <c r="E49" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F49" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="G49" s="13">
+      <c r="E49" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F49" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G49" s="12">
         <v>98.11</v>
       </c>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-      <c r="J49" s="13"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
       <c r="K49" s="1"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="15">
+      <c r="B50" s="14">
         <v>4</v>
       </c>
-      <c r="C50" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="D50" s="15">
+      <c r="C50" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D50" s="14">
         <v>0.75</v>
       </c>
-      <c r="E50" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F50" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="G50" s="13">
+      <c r="E50" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F50" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G50" s="12">
         <v>115.88</v>
       </c>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
       <c r="K50" s="1"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="B51" s="15">
+      <c r="B51" s="14">
         <v>5</v>
       </c>
-      <c r="C51" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="D51" s="15">
+      <c r="C51" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D51" s="14">
         <v>0.75</v>
       </c>
-      <c r="E51" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F51" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="G51" s="13">
+      <c r="E51" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F51" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G51" s="12">
         <v>116.88</v>
       </c>
-      <c r="H51" s="14">
+      <c r="H51" s="13">
         <f>SUM(G47:G51)/5</f>
         <v>108.35</v>
       </c>
-      <c r="I51" s="14">
+      <c r="I51" s="13">
         <f>MAX(G47:G51)</f>
         <v>116.88</v>
       </c>
-      <c r="J51" s="14">
+      <c r="J51" s="13">
         <f>MIN(G47:G51)</f>
         <v>98.11</v>
       </c>
@@ -3116,15 +3116,15 @@
       <c r="G56" s="5">
         <v>87.77</v>
       </c>
-      <c r="H56" s="14">
+      <c r="H56" s="13">
         <f>SUM(G52:G56)/5</f>
         <v>90.325999999999993</v>
       </c>
-      <c r="I56" s="14">
+      <c r="I56" s="13">
         <f>MAX(G52:G56)</f>
         <v>97.88</v>
       </c>
-      <c r="J56" s="14">
+      <c r="J56" s="13">
         <f>MIN(G52:G56)</f>
         <v>78.33</v>
       </c>
@@ -3132,133 +3132,133 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
-      <c r="B57" s="15">
-        <v>1</v>
-      </c>
-      <c r="C57" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="D57" s="15">
+      <c r="B57" s="14">
+        <v>1</v>
+      </c>
+      <c r="C57" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D57" s="14">
         <v>0.75</v>
       </c>
-      <c r="E57" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="F57" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="G57" s="13">
+      <c r="E57" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="F57" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G57" s="12">
         <v>105.44</v>
       </c>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
       <c r="K57" s="1"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
-      <c r="B58" s="15">
+      <c r="B58" s="14">
         <v>2</v>
       </c>
-      <c r="C58" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="D58" s="15">
+      <c r="C58" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D58" s="14">
         <v>0.75</v>
       </c>
-      <c r="E58" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="F58" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="G58" s="13">
+      <c r="E58" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="F58" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G58" s="12">
         <v>99</v>
       </c>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="13"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
       <c r="K58" s="1"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
-      <c r="B59" s="15">
+      <c r="B59" s="14">
         <v>3</v>
       </c>
-      <c r="C59" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="D59" s="15">
+      <c r="C59" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D59" s="14">
         <v>0.75</v>
       </c>
-      <c r="E59" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="F59" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="G59" s="13">
+      <c r="E59" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="F59" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G59" s="12">
         <v>123.66</v>
       </c>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="13"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="12"/>
       <c r="K59" s="1"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
-      <c r="B60" s="15">
+      <c r="B60" s="14">
         <v>4</v>
       </c>
-      <c r="C60" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="D60" s="15">
+      <c r="C60" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D60" s="14">
         <v>0.75</v>
       </c>
-      <c r="E60" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="F60" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="G60" s="13">
+      <c r="E60" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="F60" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G60" s="12">
         <v>112.77</v>
       </c>
-      <c r="H60" s="13"/>
-      <c r="I60" s="13"/>
-      <c r="J60" s="13"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
       <c r="K60" s="1"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
-      <c r="B61" s="15">
+      <c r="B61" s="14">
         <v>5</v>
       </c>
-      <c r="C61" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="D61" s="15">
+      <c r="C61" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D61" s="14">
         <v>0.75</v>
       </c>
-      <c r="E61" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="F61" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="G61" s="13">
+      <c r="E61" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="F61" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="G61" s="12">
         <v>96.33</v>
       </c>
-      <c r="H61" s="14">
+      <c r="H61" s="13">
         <f>SUM(G57:G61)/5</f>
         <v>107.44000000000001</v>
       </c>
-      <c r="I61" s="14">
+      <c r="I61" s="13">
         <f>MAX(G57:G61)</f>
         <v>123.66</v>
       </c>
-      <c r="J61" s="14">
+      <c r="J61" s="13">
         <f>MIN(G57:G61)</f>
         <v>96.33</v>
       </c>
@@ -3384,15 +3384,15 @@
       <c r="G66" s="5">
         <v>107.55</v>
       </c>
-      <c r="H66" s="14">
+      <c r="H66" s="13">
         <f>SUM(G62:G66)/5</f>
         <v>119.90799999999999</v>
       </c>
-      <c r="I66" s="14">
+      <c r="I66" s="13">
         <f>MAX(G62:G66)</f>
         <v>136</v>
       </c>
-      <c r="J66" s="14">
+      <c r="J66" s="13">
         <f>MIN(G62:G66)</f>
         <v>107.55</v>
       </c>
@@ -3401,7 +3401,7 @@
       </c>
     </row>
     <row r="67" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="K67" s="18" t="s">
+      <c r="K67" s="17" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3433,7 +3433,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>18</v>
@@ -3453,8 +3453,8 @@
       <c r="G1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="16" t="s">
-        <v>31</v>
+      <c r="H1" s="15" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3600,7 +3600,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>18</v>
@@ -3620,8 +3620,8 @@
       <c r="G9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="16" t="s">
-        <v>29</v>
+      <c r="H9" s="15" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3774,7 +3774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD4186B-45AF-4C92-9836-21427EBF0B8E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>

</xml_diff>